<commit_message>
Add Name on Menu
</commit_message>
<xml_diff>
--- a/Grille de correction - Gabarit.xlsx
+++ b/Grille de correction - Gabarit.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasbonnardot/Desktop/Laval/DevWeb/Projet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasbonnardot/Desktop/Laval/DevWeb/Projet/team13/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="540" windowWidth="28560" windowHeight="17380" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="540" windowWidth="28560" windowHeight="17380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Livrable 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Livrable 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Livrable 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Feuil1" sheetId="4" r:id="rId2"/>
+    <sheet name="Livrable 2" sheetId="2" r:id="rId3"/>
+    <sheet name="Livrable 3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="128">
   <si>
     <t>Livrable 3</t>
   </si>
@@ -323,13 +324,100 @@
   </si>
   <si>
     <t>present</t>
+  </si>
+  <si>
+    <t>Developpement Web</t>
+  </si>
+  <si>
+    <t>Partiel 1</t>
+  </si>
+  <si>
+    <t>Partiel 2</t>
+  </si>
+  <si>
+    <t>Lab 1</t>
+  </si>
+  <si>
+    <t>Lab 2</t>
+  </si>
+  <si>
+    <t>Lab 3</t>
+  </si>
+  <si>
+    <t>Lab 4</t>
+  </si>
+  <si>
+    <t>Lab 5</t>
+  </si>
+  <si>
+    <t>Lab 6</t>
+  </si>
+  <si>
+    <t>Lab 7</t>
+  </si>
+  <si>
+    <t>Lab 8</t>
+  </si>
+  <si>
+    <t>Lab 9</t>
+  </si>
+  <si>
+    <t>Lab 10</t>
+  </si>
+  <si>
+    <t>Lab 11</t>
+  </si>
+  <si>
+    <t>Livrable 4</t>
+  </si>
+  <si>
+    <t>AutoEvaluation</t>
+  </si>
+  <si>
+    <t>Algorithmique</t>
+  </si>
+  <si>
+    <t>TP1</t>
+  </si>
+  <si>
+    <t>TP2</t>
+  </si>
+  <si>
+    <t>TP3</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Intelligence Artificielle</t>
+  </si>
+  <si>
+    <t>Mon app</t>
+  </si>
+  <si>
+    <t>Jeu intelligent</t>
+  </si>
+  <si>
+    <t>SBC</t>
+  </si>
+  <si>
+    <t>TALN</t>
+  </si>
+  <si>
+    <t>Particip</t>
+  </si>
+  <si>
+    <t>Evaluation</t>
+  </si>
+  <si>
+    <t>Genie Logiciel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -346,6 +434,11 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -372,10 +465,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -394,13 +488,444 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -675,7 +1200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1304,6 +1829,794 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:O34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" s="13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B6" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="10">
+        <v>36</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="F6">
+        <f>C6/D6*E6</f>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="J6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K6">
+        <v>66</v>
+      </c>
+      <c r="L6" s="15">
+        <v>100</v>
+      </c>
+      <c r="M6" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="N6">
+        <f>K6/L6*M6</f>
+        <v>0.13200000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B7" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" ref="F7:F12" si="0">C7/D7*E7</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="J7" t="s">
+        <v>101</v>
+      </c>
+      <c r="L7" s="15">
+        <v>100</v>
+      </c>
+      <c r="M7" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="N7" s="10">
+        <f t="shared" ref="N7:N22" si="1">K7/L7*M7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="17">
+        <v>11.35</v>
+      </c>
+      <c r="D8">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="0"/>
+        <v>0.11350000000000002</v>
+      </c>
+      <c r="H8" s="17">
+        <f>C8+C9+C10+C11</f>
+        <v>24.85</v>
+      </c>
+      <c r="I8">
+        <f>D8+D9+D11+D10</f>
+        <v>59</v>
+      </c>
+      <c r="J8" t="s">
+        <v>102</v>
+      </c>
+      <c r="K8">
+        <v>100</v>
+      </c>
+      <c r="L8" s="15">
+        <v>100</v>
+      </c>
+      <c r="M8" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N8" s="10">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="10">
+        <v>13.5</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" si="0"/>
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9">
+        <f>H8/I8*100</f>
+        <v>42.118644067796609</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="K9" s="10">
+        <v>100</v>
+      </c>
+      <c r="L9" s="15">
+        <v>100</v>
+      </c>
+      <c r="M9" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N9" s="10">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B10" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="J10" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K10" s="10">
+        <v>100</v>
+      </c>
+      <c r="L10" s="15">
+        <v>100</v>
+      </c>
+      <c r="M10" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N10" s="10">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B11" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="J11" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="K11" s="10">
+        <v>100</v>
+      </c>
+      <c r="L11" s="15">
+        <v>100</v>
+      </c>
+      <c r="M11" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N11" s="10">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B12" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="G12" s="18" t="str">
+        <f>IF(F13&lt;D4,"manque","plus de")</f>
+        <v>manque</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="J12" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K12" s="10">
+        <v>100</v>
+      </c>
+      <c r="L12" s="15">
+        <v>100</v>
+      </c>
+      <c r="M12" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N12" s="10">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="F13" s="14">
+        <f>SUM(F6:F12)</f>
+        <v>0.33050000000000002</v>
+      </c>
+      <c r="G13" s="16">
+        <f>ABS(F13-D4)</f>
+        <v>0.26949999999999996</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="K13" s="10">
+        <v>100</v>
+      </c>
+      <c r="L13" s="15">
+        <v>100</v>
+      </c>
+      <c r="M13" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N13" s="10">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="J14" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="K14" s="10">
+        <v>50</v>
+      </c>
+      <c r="L14" s="15">
+        <v>100</v>
+      </c>
+      <c r="M14" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N14" s="10">
+        <f t="shared" si="1"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="J15" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="K15" s="10">
+        <v>100</v>
+      </c>
+      <c r="L15" s="15">
+        <v>100</v>
+      </c>
+      <c r="M15" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N15" s="10">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="J16" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="L16" s="15">
+        <v>100</v>
+      </c>
+      <c r="M16" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N16" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="J17" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="L17" s="15">
+        <v>100</v>
+      </c>
+      <c r="M17" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N17" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="J18" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="L18" s="15">
+        <v>100</v>
+      </c>
+      <c r="M18" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N18" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="J19" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K19">
+        <v>93</v>
+      </c>
+      <c r="L19" s="15">
+        <v>100</v>
+      </c>
+      <c r="M19" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="N19" s="10">
+        <f t="shared" si="1"/>
+        <v>9.3000000000000013E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="J20" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20">
+        <v>76</v>
+      </c>
+      <c r="L20" s="15">
+        <v>100</v>
+      </c>
+      <c r="M20" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="N20" s="10">
+        <f t="shared" si="1"/>
+        <v>7.6000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="J21" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21" s="15">
+        <v>100</v>
+      </c>
+      <c r="M21" s="13">
+        <v>0.24</v>
+      </c>
+      <c r="N21" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="J22" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="L22" s="15">
+        <v>100</v>
+      </c>
+      <c r="M22" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="N22" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="18" t="str">
+        <f>IF(N23&lt;L4,"manque","plus de")</f>
+        <v>manque</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="M23" s="13">
+        <f>SUM(M6:M22)</f>
+        <v>1</v>
+      </c>
+      <c r="N23" s="16">
+        <f>SUM(N6:N22)</f>
+        <v>0.37600000000000011</v>
+      </c>
+      <c r="O23" s="16">
+        <f>ABS(N23-L4)</f>
+        <v>0.12399999999999989</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B25" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="J25" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="K25" s="10"/>
+      <c r="L25" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B27" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="10">
+        <v>77</v>
+      </c>
+      <c r="D27" s="15">
+        <v>100</v>
+      </c>
+      <c r="E27" s="13">
+        <v>0.35</v>
+      </c>
+      <c r="F27" s="10">
+        <f>C27/D27*E27</f>
+        <v>0.26949999999999996</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="K27" s="10">
+        <v>88</v>
+      </c>
+      <c r="L27" s="15">
+        <v>100</v>
+      </c>
+      <c r="M27" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="N27" s="10">
+        <f>K27/L27*M27</f>
+        <v>0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B28" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="15">
+        <v>100</v>
+      </c>
+      <c r="E28" s="13">
+        <v>0.35</v>
+      </c>
+      <c r="F28" s="10">
+        <f t="shared" ref="F28:F33" si="2">C28/D28*E28</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K28" s="10"/>
+      <c r="L28" s="15">
+        <v>100</v>
+      </c>
+      <c r="M28" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="N28" s="10">
+        <f t="shared" ref="N28:N32" si="3">K28/L28*M28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B29" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="10">
+        <v>95</v>
+      </c>
+      <c r="D29" s="15">
+        <v>100</v>
+      </c>
+      <c r="E29" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="F29" s="10">
+        <f t="shared" si="2"/>
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="K29" s="10">
+        <v>98</v>
+      </c>
+      <c r="L29" s="15">
+        <v>100</v>
+      </c>
+      <c r="M29" s="13">
+        <v>0.08</v>
+      </c>
+      <c r="N29" s="10">
+        <f t="shared" si="3"/>
+        <v>7.8399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B30" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="10">
+        <v>90</v>
+      </c>
+      <c r="D30" s="15">
+        <v>100</v>
+      </c>
+      <c r="E30" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="F30" s="10">
+        <f t="shared" si="2"/>
+        <v>4.5000000000000005E-2</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="K30" s="10">
+        <v>95</v>
+      </c>
+      <c r="L30" s="15">
+        <v>100</v>
+      </c>
+      <c r="M30" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="N30" s="10">
+        <f t="shared" si="3"/>
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B31" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="10">
+        <v>100</v>
+      </c>
+      <c r="D31" s="15">
+        <v>100</v>
+      </c>
+      <c r="E31" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="F31" s="10">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="K31" s="10"/>
+      <c r="L31" s="15">
+        <v>100</v>
+      </c>
+      <c r="M31" s="13">
+        <v>0.12</v>
+      </c>
+      <c r="N31" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B32" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="15">
+        <v>100</v>
+      </c>
+      <c r="E32" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="F32" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="K32" s="10"/>
+      <c r="L32" s="15">
+        <v>100</v>
+      </c>
+      <c r="M32" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="N32" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O32" s="18" t="str">
+        <f>IF(N33&lt;L25,"manque","plus de")</f>
+        <v>manque</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B33" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="15">
+        <v>100</v>
+      </c>
+      <c r="E33" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="F33" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="18" t="str">
+        <f>IF(F34&lt;D25,"manque","plus de")</f>
+        <v>manque</v>
+      </c>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="13">
+        <f>SUM(M27:M32)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="N33" s="16">
+        <f>SUM(N27:N32)</f>
+        <v>0.43740000000000001</v>
+      </c>
+      <c r="O33" s="16">
+        <f>ABS(N33-L25)</f>
+        <v>0.16259999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="13">
+        <f>SUM(E27:E33)</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="16">
+        <f>SUM(F27:F33)</f>
+        <v>0.45949999999999991</v>
+      </c>
+      <c r="G34" s="16">
+        <f>ABS(F34-D25)</f>
+        <v>4.0500000000000091E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="N23">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="lessThan">
+      <formula>$L$4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="greaterThan">
+      <formula>$L$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N33">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="lessThan">
+      <formula>$L$25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="greaterThan">
+      <formula>$L$25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F34">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="lessThan">
+      <formula>$D$25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
+      <formula>$D$25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="greaterThan">
+      <formula>$D$4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
+      <formula>$D$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1379,10 +2692,10 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
@@ -1406,10 +2719,10 @@
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
@@ -1460,10 +2773,10 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
@@ -1493,10 +2806,10 @@
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
@@ -1520,10 +2833,10 @@
       </c>
     </row>
     <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
@@ -1553,10 +2866,10 @@
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
@@ -1580,10 +2893,10 @@
       </c>
     </row>
     <row r="28" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="12"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
@@ -1604,10 +2917,10 @@
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="11"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5">
         <v>5</v>
@@ -1739,7 +3052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB48"/>
   <sheetViews>
@@ -1802,10 +3115,10 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
@@ -1829,10 +3142,10 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
@@ -2046,10 +3359,10 @@
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="12"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
@@ -2093,10 +3406,10 @@
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="11"/>
+      <c r="C33" s="12"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
     </row>

</xml_diff>